<commit_message>
Made all plots that I think are necessary so far, part 1
I believe that I've conducted all of the statistical analyses that are good enough for my thesis, and I've made all the necessary plots (as far as I believe). That includes the linear regression of Km vs Vmax to test hypothesis 1. And, gotta say, hypothesis 1 is essentially validated. Yay.
</commit_message>
<xml_diff>
--- a/Statistical analyses/ANOVA, updated with Tukey.xlsx
+++ b/Statistical analyses/ANOVA, updated with Tukey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LMAOXD\Documents\UCI undergrad\Bio-ESS 199\Microbial enzyme activity in leaf litter\Statistical analyses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A3DD85-8FDF-4D24-AA91-B752D07829BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A58EC35F-F97A-4452-92EC-277A4E3A49EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -449,7 +449,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -613,7 +613,7 @@
         <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Created CLDs for Tukey's results on litter chemistry
After looking through these compact letter displays (CLDs), I saw that some main effects/interactions that were significant under ANOVAs were insignificant under Tukey post-hoc. As  result, I deleted the Tukey results for these main effects/interactions.

Now, I can start making boxplots.
</commit_message>
<xml_diff>
--- a/Statistical analyses/ANOVA, updated with Tukey.xlsx
+++ b/Statistical analyses/ANOVA, updated with Tukey.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LMAOXD\Documents\UCI undergrad\Bio-ESS 199\Microbial-enzyme-activity-in-leaf-litter\Statistical analyses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50A57801-5F87-4381-ADAC-E1F452B86A41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3FF35C-E33E-4F6F-8180-986F58874369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11532" yWindow="4116" windowWidth="17280" windowHeight="9420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vmax" sheetId="1" r:id="rId1"/>
     <sheet name="Km" sheetId="3" r:id="rId2"/>
+    <sheet name="litterChemistry" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="31">
   <si>
     <t>Enzyme</t>
   </si>
@@ -98,6 +99,27 @@
   </si>
   <si>
     <t>MANOVA</t>
+  </si>
+  <si>
+    <t>functionalGroup</t>
+  </si>
+  <si>
+    <t>glycosidicBond</t>
+  </si>
+  <si>
+    <t>C_O_stretching</t>
+  </si>
+  <si>
+    <t>carboEster</t>
+  </si>
+  <si>
+    <t>lipid</t>
+  </si>
+  <si>
+    <t>alkane</t>
+  </si>
+  <si>
+    <t>amide</t>
   </si>
 </sst>
 </file>
@@ -147,7 +169,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -155,17 +177,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,7 +488,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -742,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2014A953-EC86-410A-AF55-A076AABF3B1D}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1021,4 +1060,211 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{379B1082-EA44-4F9E-B0F3-6D60E21C5FD2}">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Tukey's post-hoc of CAZyme domain data
Performed Tukey's post-hoc on CAZyme domain data. I may perform additional Tukey's test on other main effects or interactions on the CAZyme domain data.
</commit_message>
<xml_diff>
--- a/Statistical analyses/ANOVA, updated with Tukey.xlsx
+++ b/Statistical analyses/ANOVA, updated with Tukey.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LMAOXD\Documents\UCI undergrad\Bio-ESS 199\Microbial-enzyme-activity-in-leaf-litter\Statistical analyses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F709454-C39B-4009-BDF1-EABD3B5D8A20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38CEA0F6-0647-4A97-AF55-751A40B1C692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vmax" sheetId="1" r:id="rId1"/>
     <sheet name="Km" sheetId="3" r:id="rId2"/>
     <sheet name="litterChemistry" sheetId="4" r:id="rId3"/>
+    <sheet name="CAZyme domains" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="50">
   <si>
     <t>Enzyme</t>
   </si>
@@ -132,6 +133,51 @@
   </si>
   <si>
     <t>amide2</t>
+  </si>
+  <si>
+    <t>Substrate</t>
+  </si>
+  <si>
+    <t>Hemicellulose</t>
+  </si>
+  <si>
+    <t>Lignin</t>
+  </si>
+  <si>
+    <t>Polysaccharide</t>
+  </si>
+  <si>
+    <t>Oligosaccharides</t>
+  </si>
+  <si>
+    <t>Cell_wall</t>
+  </si>
+  <si>
+    <t>Inulin</t>
+  </si>
+  <si>
+    <t>Starch</t>
+  </si>
+  <si>
+    <t>Trehalose</t>
+  </si>
+  <si>
+    <t>Cellulose</t>
+  </si>
+  <si>
+    <t>Pectin</t>
+  </si>
+  <si>
+    <t>Glycogen</t>
+  </si>
+  <si>
+    <t>Peptidoglycan</t>
+  </si>
+  <si>
+    <t>Chitin</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -1079,8 +1125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{379B1082-EA44-4F9E-B0F3-6D60E21C5FD2}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1384,4 +1430,419 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E3897FB-34D0-4D95-9381-F39E8F15B0FF}">
+  <dimension ref="A1:H15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>